<commit_message>
prg Mon Dec 29 08:15:55 PM CET 2025
</commit_message>
<xml_diff>
--- a/public/routers/A6_Sistema_FV/A60_Comun/FV00_Tramitación_instalaciones_de_autoconsumo.xlsx
+++ b/public/routers/A6_Sistema_FV/A60_Comun/FV00_Tramitación_instalaciones_de_autoconsumo.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Parametros" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="ParametrosAutoconsumo" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,79 +453,500 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Años análisis</t>
+          <t>Potencia instalada</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>años</t>
+          <t>kW</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Tasa interés</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>6.2</v>
+          <t>Tensión de conexión</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>BT;MT;AT</t>
+        </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>%</t>
+          <t>-</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>k Inversión inicial</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>1.1</v>
+          <t>Modalidad autoconsumo</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Con excedentes y compensación;Sin excedentes;Con excedentes sin compensación</t>
+        </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>k €/kWp</t>
+          <t>-</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Gastos operativos</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>5000</v>
+          <t>Ubicación paneles</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Cubierta coplanar;Cubierta no coplanar;Sobre pergola;Suelo;Fachada</t>
+        </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>€</t>
+          <t>-</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Ingresos fijos</t>
+          <t>Tipo de suelo</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
+          <t>Urbano;No urbano</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Área servidumbre aeronáutica</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>No;Sí</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Superficie aproximada</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>60</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>m²</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Distancia a red eléctrica</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>50</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Número de consumidores</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Tipo instalación</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Individual;Colectiva</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Tecnología generación</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Fotovoltaica;Eólica</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Comunidad Autónoma</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Madrid;Cataluña;Andalucía;Valencia;País Vasco;Castilla y León;Castilla-La Mancha;Galicia;Aragón;Murcia;Extremadura;Navarra;Asturias;Cantabria;La Rioja;Baleares;Canarias</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Municipio</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Coslada;Madrid;Barcelona;Sevilla;Valencia;Zaragoza;Bilbao</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Distribuidora eléctrica</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>i-DE;e-distribución;UFD;Viesgo;Other</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Comercializadora actual</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Endesa;Iberdrola;Naturgy;EDP;Repsol;Total;Other</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Titular contrato</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Propietario;Arrendatario;Comunidad</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Documentación catastral</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Completa;Incompleta;No disponible</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Permiso comunidad propietarios</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Obtenido;Pendiente;No requerido</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Tipo cubierta</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Plana;Inclinada;Mixta</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Material cubierta</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Ligera;Pesada;Mixta</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Necesita refuerzo estructural</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>No;Sí</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Acceso a cubierta</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Fácil;Difícil;Muy difícil</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Orientación paneles</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Sur;Sureste;Suroeste;Este;Oeste;Norte</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Sombras presentes</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Nulas;Bajas;Moderadas;Altas</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Uso edificio</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Residencial;Industrial;Comercial;Administrativo</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Subvención solicitada</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>No;Sí</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Financiación necesaria</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>No;Sí</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Estado documentación</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Completa;Parcial;Por iniciar</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Experiencia tramitación</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Ninguna;Básica;Avanzada</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>coordenadas</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
           <t>{'coordenadas': [['lat', 37.00255267215955], ['lon', -5.313171409070493]]}</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>€</t>
-        </is>
-      </c>
+      <c r="C31" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>